<commit_message>
4/23 updates, add new data from NY, WA and use state controls
- Use updated data from NY and WA on job losses by industyr
- Also use BLS advance claims to set up state controls for each state. This allows us to up/down weight the job loss esimates of each state to be in line with the preliminary BLS estimates and therefore more accurate
</commit_message>
<xml_diff>
--- a/data/raw-data/small/initial-claims-bls-state.xlsx
+++ b/data/raw-data/small/initial-claims-bls-state.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\GMacDonald\Documents\covid-neighborhood-job-analysis\data\raw-data\small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB64A7E-2969-4776-934E-3637E6170E11}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19E550C-154C-436F-B07F-4D0B95F75B26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="4020" windowWidth="9600" windowHeight="3585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="#,##0;#,##0"/>
+    <numFmt numFmtId="165" formatCode="###0;###0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,7 +211,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
@@ -232,12 +254,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,18 +616,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:P56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,10 +644,19 @@
       <c r="E1" s="1">
         <v>43932</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F1" s="1">
+        <v>43939</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -620,12 +670,21 @@
         <v>106739</v>
       </c>
       <c r="E2">
-        <v>91079</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>77515</v>
+      </c>
+      <c r="F2">
+        <v>65431</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -639,12 +698,21 @@
         <v>14590</v>
       </c>
       <c r="E3">
-        <v>12752</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>12007</v>
+      </c>
+      <c r="F3">
+        <v>13027</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -658,12 +726,21 @@
         <v>62086</v>
       </c>
       <c r="E4">
-        <v>34635</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>35629</v>
+      </c>
+      <c r="F4">
+        <v>24236</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -677,12 +754,21 @@
         <v>132428</v>
       </c>
       <c r="E5">
-        <v>97784</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>98531</v>
+      </c>
+      <c r="F5">
+        <v>71843</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -696,12 +782,21 @@
         <v>918814</v>
       </c>
       <c r="E6">
-        <v>660966</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>655472</v>
+      </c>
+      <c r="F6">
+        <v>533568</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -715,12 +810,21 @@
         <v>46326</v>
       </c>
       <c r="E7">
-        <v>105073</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>104572</v>
+      </c>
+      <c r="F7">
+        <v>68667</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -734,12 +838,21 @@
         <v>33464</v>
       </c>
       <c r="E8">
-        <v>33962</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34050</v>
+      </c>
+      <c r="F8">
+        <v>102757</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -753,12 +866,21 @@
         <v>18851</v>
       </c>
       <c r="E9">
-        <v>13272</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>13258</v>
+      </c>
+      <c r="F9">
+        <v>9294</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -772,12 +894,21 @@
         <v>15329</v>
       </c>
       <c r="E10">
-        <v>9904</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9974</v>
+      </c>
+      <c r="F10">
+        <v>8591</v>
+      </c>
+      <c r="H10" s="8"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -791,12 +922,21 @@
         <v>169885</v>
       </c>
       <c r="E11">
-        <v>181293</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>180419</v>
+      </c>
+      <c r="F11">
+        <v>505137</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -810,12 +950,21 @@
         <v>390132</v>
       </c>
       <c r="E12">
-        <v>317526</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>319581</v>
+      </c>
+      <c r="F12">
+        <v>243677</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -829,12 +978,21 @@
         <v>53101</v>
       </c>
       <c r="E13">
-        <v>34693</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>34717</v>
+      </c>
+      <c r="F13">
+        <v>26477</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -848,12 +1006,21 @@
         <v>30904</v>
       </c>
       <c r="E14">
-        <v>17817</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18531</v>
+      </c>
+      <c r="F14">
+        <v>12456</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -867,12 +1034,21 @@
         <v>201041</v>
       </c>
       <c r="E15">
-        <v>141049</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>141160</v>
+      </c>
+      <c r="F15">
+        <v>102736</v>
+      </c>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -886,12 +1062,21 @@
         <v>127010</v>
       </c>
       <c r="E16">
-        <v>118184</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>113755</v>
+      </c>
+      <c r="F16">
+        <v>75483</v>
+      </c>
+      <c r="H16" s="5"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -905,12 +1090,21 @@
         <v>64194</v>
       </c>
       <c r="E17">
-        <v>46356</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>43889</v>
+      </c>
+      <c r="F17">
+        <v>27912</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -924,12 +1118,21 @@
         <v>49306</v>
       </c>
       <c r="E18">
-        <v>30769</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>29873</v>
+      </c>
+      <c r="F18">
+        <v>31920</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -943,12 +1146,21 @@
         <v>117575</v>
       </c>
       <c r="E19">
-        <v>115763</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>116277</v>
+      </c>
+      <c r="F19">
+        <v>103548</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -962,12 +1174,21 @@
         <v>100621</v>
       </c>
       <c r="E20">
-        <v>80045</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>79653</v>
+      </c>
+      <c r="F20">
+        <v>92039</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -981,12 +1202,21 @@
         <v>30910</v>
       </c>
       <c r="E21">
-        <v>13273</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>13488</v>
+      </c>
+      <c r="F21">
+        <v>11446</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1000,12 +1230,21 @@
         <v>109496</v>
       </c>
       <c r="E22">
-        <v>60823</v>
-      </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62904</v>
+      </c>
+      <c r="F22">
+        <v>46676</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1019,12 +1258,21 @@
         <v>139647</v>
       </c>
       <c r="E23">
-        <v>103040</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>103813</v>
+      </c>
+      <c r="F23">
+        <v>80345</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1038,12 +1286,21 @@
         <v>388554</v>
       </c>
       <c r="E24">
-        <v>219320</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>222207</v>
+      </c>
+      <c r="F24">
+        <v>134119</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1057,12 +1314,21 @@
         <v>110260</v>
       </c>
       <c r="E25">
-        <v>89634</v>
-      </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>93133</v>
+      </c>
+      <c r="F25">
+        <v>74873</v>
+      </c>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1076,12 +1342,21 @@
         <v>45852</v>
       </c>
       <c r="E26">
-        <v>46160</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>45748</v>
+      </c>
+      <c r="F26">
+        <v>35843</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1095,12 +1370,21 @@
         <v>91458</v>
       </c>
       <c r="E27">
-        <v>95785</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>102126</v>
+      </c>
+      <c r="F27">
+        <v>52678</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1114,12 +1398,21 @@
         <v>21244</v>
       </c>
       <c r="E28">
-        <v>13437</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>14275</v>
+      </c>
+      <c r="F28">
+        <v>10509</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1133,12 +1426,21 @@
         <v>137422</v>
       </c>
       <c r="E29">
-        <v>137934</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>140155</v>
+      </c>
+      <c r="F29">
+        <v>104515</v>
+      </c>
+      <c r="H29" s="5"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1152,12 +1454,21 @@
         <v>15125</v>
       </c>
       <c r="E30">
-        <v>10378</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9502</v>
+      </c>
+      <c r="F30">
+        <v>9042</v>
+      </c>
+      <c r="H30" s="5"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1171,12 +1482,21 @@
         <v>27054</v>
       </c>
       <c r="E31">
-        <v>16391</v>
-      </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>16279</v>
+      </c>
+      <c r="F31">
+        <v>12340</v>
+      </c>
+      <c r="H31" s="5"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1190,12 +1510,21 @@
         <v>39202</v>
       </c>
       <c r="E32">
-        <v>23936</v>
-      </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>25273</v>
+      </c>
+      <c r="F32">
+        <v>19110</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1209,12 +1538,21 @@
         <v>214836</v>
       </c>
       <c r="E33">
-        <v>140600</v>
-      </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>141420</v>
+      </c>
+      <c r="F33">
+        <v>139277</v>
+      </c>
+      <c r="H33" s="5"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1228,12 +1566,21 @@
         <v>26132</v>
       </c>
       <c r="E34">
-        <v>19494</v>
-      </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>19043</v>
+      </c>
+      <c r="F34">
+        <v>13338</v>
+      </c>
+      <c r="H34" s="5"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1247,12 +1594,21 @@
         <v>79285</v>
       </c>
       <c r="E35">
-        <v>60180</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>58641</v>
+      </c>
+      <c r="F35">
+        <v>40909</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1266,12 +1622,21 @@
         <v>344451</v>
       </c>
       <c r="E36">
-        <v>395949</v>
-      </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>394701</v>
+      </c>
+      <c r="F36">
+        <v>204716</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1285,12 +1650,21 @@
         <v>226191</v>
       </c>
       <c r="E37">
-        <v>157218</v>
-      </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>159317</v>
+      </c>
+      <c r="F37">
+        <v>108801</v>
+      </c>
+      <c r="H37" s="5"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1304,12 +1678,21 @@
         <v>60534</v>
       </c>
       <c r="E38">
-        <v>48977</v>
-      </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>54481</v>
+      </c>
+      <c r="F38">
+        <v>40297</v>
+      </c>
+      <c r="H38" s="5"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1323,12 +1706,21 @@
         <v>62788</v>
       </c>
       <c r="E39">
-        <v>50930</v>
-      </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>54581</v>
+      </c>
+      <c r="F39">
+        <v>35101</v>
+      </c>
+      <c r="H39" s="8"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1342,12 +1734,21 @@
         <v>277640</v>
       </c>
       <c r="E40">
-        <v>238357</v>
-      </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="3"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>234868</v>
+      </c>
+      <c r="F40">
+        <v>198081</v>
+      </c>
+      <c r="H40" s="5"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1361,12 +1762,21 @@
         <v>66555</v>
       </c>
       <c r="E41">
-        <v>41829</v>
-      </c>
-      <c r="H41" s="2"/>
-      <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42074</v>
+      </c>
+      <c r="F41">
+        <v>26248</v>
+      </c>
+      <c r="H41" s="5"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="5"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1380,12 +1790,21 @@
         <v>28243</v>
       </c>
       <c r="E42">
-        <v>22805</v>
-      </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22509</v>
+      </c>
+      <c r="F42">
+        <v>17578</v>
+      </c>
+      <c r="H42" s="5"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1399,12 +1818,21 @@
         <v>86573</v>
       </c>
       <c r="E43">
-        <v>87686</v>
-      </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="3"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <v>89147</v>
+      </c>
+      <c r="F43">
+        <v>73116</v>
+      </c>
+      <c r="H43" s="5"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1418,12 +1846,21 @@
         <v>8138</v>
       </c>
       <c r="E44">
-        <v>6152</v>
-      </c>
-      <c r="H44" s="2"/>
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <v>6359</v>
+      </c>
+      <c r="F44">
+        <v>5128</v>
+      </c>
+      <c r="H44" s="5"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1437,12 +1874,21 @@
         <v>112186</v>
       </c>
       <c r="E45">
-        <v>74772</v>
-      </c>
-      <c r="H45" s="2"/>
-      <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>71887</v>
+      </c>
+      <c r="F45">
+        <v>68968</v>
+      </c>
+      <c r="H45" s="5"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1456,12 +1902,21 @@
         <v>315167</v>
       </c>
       <c r="E46">
-        <v>273567</v>
-      </c>
-      <c r="H46" s="2"/>
-      <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+        <v>274257</v>
+      </c>
+      <c r="F46">
+        <v>280406</v>
+      </c>
+      <c r="H46" s="5"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1475,12 +1930,21 @@
         <v>33040</v>
       </c>
       <c r="E47">
-        <v>24171</v>
-      </c>
-      <c r="H47" s="2"/>
-      <c r="I47" s="3"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24515</v>
+      </c>
+      <c r="F47">
+        <v>19751</v>
+      </c>
+      <c r="H47" s="5"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1494,12 +1958,21 @@
         <v>16474</v>
       </c>
       <c r="E48">
-        <v>9478</v>
-      </c>
-      <c r="H48" s="2"/>
-      <c r="I48" s="4"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9662</v>
+      </c>
+      <c r="F48">
+        <v>6434</v>
+      </c>
+      <c r="H48" s="5"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="7"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1513,12 +1986,21 @@
         <v>72</v>
       </c>
       <c r="E49">
-        <v>3</v>
-      </c>
-      <c r="H49" s="2"/>
-      <c r="I49" s="3"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="H49" s="5"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1532,12 +2014,21 @@
         <v>147369</v>
       </c>
       <c r="E50">
-        <v>106723</v>
-      </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="3"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>104619</v>
+      </c>
+      <c r="F50">
+        <v>84387</v>
+      </c>
+      <c r="H50" s="5"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="6"/>
+      <c r="P50" s="6"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1551,12 +2042,21 @@
         <v>171252</v>
       </c>
       <c r="E51">
-        <v>150516</v>
-      </c>
-      <c r="H51" s="2"/>
-      <c r="I51" s="3"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+        <v>144455</v>
+      </c>
+      <c r="F51">
+        <v>89105</v>
+      </c>
+      <c r="H51" s="5"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+      <c r="P51" s="6"/>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1570,12 +2070,21 @@
         <v>14494</v>
       </c>
       <c r="E52">
-        <v>14595</v>
-      </c>
-      <c r="H52" s="2"/>
-      <c r="I52" s="3"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+        <v>14944</v>
+      </c>
+      <c r="F52">
+        <v>46251</v>
+      </c>
+      <c r="H52" s="5"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="5"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+      <c r="P52" s="6"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1589,12 +2098,21 @@
         <v>104823</v>
       </c>
       <c r="E53">
-        <v>69884</v>
-      </c>
-      <c r="H53" s="2"/>
-      <c r="I53" s="3"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+        <v>70000</v>
+      </c>
+      <c r="F53">
+        <v>55886</v>
+      </c>
+      <c r="H53" s="5"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1608,8 +2126,26 @@
         <v>6543</v>
       </c>
       <c r="E54">
-        <v>4904</v>
-      </c>
+        <v>5794</v>
+      </c>
+      <c r="F54">
+        <v>3321</v>
+      </c>
+      <c r="I54" s="2"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="4"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K55" s="2"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="4"/>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K56" s="2"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Run scripts 1 and 2 for 4/25 data
</commit_message>
<xml_diff>
--- a/data/raw-data/small/initial-claims-bls-state.xlsx
+++ b/data/raw-data/small/initial-claims-bls-state.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\GMacDonald\Documents\covid-neighborhood-job-analysis\data\raw-data\small\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anarayanan\Documents\GitHub\covid-neighborhood-job-analysis\data\raw-data\small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19E550C-154C-436F-B07F-4D0B95F75B26}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -197,35 +196,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0;#,##0"/>
     <numFmt numFmtId="165" formatCode="###0;###0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="8"/>
@@ -254,28 +236,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -615,20 +582,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,16 +615,13 @@
       <c r="F1" s="1">
         <v>43939</v>
       </c>
-      <c r="H1" s="8"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G1" s="1">
+        <v>43946</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -673,18 +638,15 @@
         <v>77515</v>
       </c>
       <c r="F2">
-        <v>65431</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>66432</v>
+      </c>
+      <c r="G2">
+        <v>64170</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -701,18 +663,15 @@
         <v>12007</v>
       </c>
       <c r="F3">
-        <v>13027</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>12201</v>
+      </c>
+      <c r="G3">
+        <v>1187</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -729,18 +688,15 @@
         <v>35629</v>
       </c>
       <c r="F4">
-        <v>24236</v>
-      </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>25404</v>
+      </c>
+      <c r="G4">
+        <v>16745</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -757,18 +713,15 @@
         <v>98531</v>
       </c>
       <c r="F5">
-        <v>71843</v>
-      </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>72457</v>
+      </c>
+      <c r="G5">
+        <v>52098</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -785,18 +738,15 @@
         <v>655472</v>
       </c>
       <c r="F6">
-        <v>533568</v>
-      </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>528360</v>
+      </c>
+      <c r="G6">
+        <v>328042</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -813,18 +763,15 @@
         <v>104572</v>
       </c>
       <c r="F7">
-        <v>68667</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>67639</v>
+      </c>
+      <c r="G7">
+        <v>38367</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -841,18 +788,15 @@
         <v>34050</v>
       </c>
       <c r="F8">
-        <v>102757</v>
-      </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>102808</v>
+      </c>
+      <c r="G8">
+        <v>33037</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -869,18 +813,15 @@
         <v>13258</v>
       </c>
       <c r="F9">
-        <v>9294</v>
-      </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>9446</v>
+      </c>
+      <c r="G9">
+        <v>7754</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -897,18 +838,15 @@
         <v>9974</v>
       </c>
       <c r="F10">
-        <v>8591</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>8639</v>
+      </c>
+      <c r="G10">
+        <v>8158</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -925,18 +863,15 @@
         <v>180419</v>
       </c>
       <c r="F11">
-        <v>505137</v>
-      </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>506670</v>
+      </c>
+      <c r="G11">
+        <v>432465</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -953,18 +888,15 @@
         <v>319581</v>
       </c>
       <c r="F12">
-        <v>243677</v>
-      </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>247003</v>
+      </c>
+      <c r="G12">
+        <v>264818</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -981,18 +913,15 @@
         <v>34717</v>
       </c>
       <c r="F13">
-        <v>26477</v>
-      </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>26591</v>
+      </c>
+      <c r="G13">
+        <v>22615</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1009,18 +938,15 @@
         <v>18531</v>
       </c>
       <c r="F14">
-        <v>12456</v>
-      </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>13023</v>
+      </c>
+      <c r="G14">
+        <v>8268</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1037,18 +963,15 @@
         <v>141160</v>
       </c>
       <c r="F15">
-        <v>102736</v>
-      </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>102936</v>
+      </c>
+      <c r="G15">
+        <v>81245</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1065,18 +988,15 @@
         <v>113755</v>
       </c>
       <c r="F16">
-        <v>75483</v>
-      </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+        <v>72756</v>
+      </c>
+      <c r="G16">
+        <v>57397</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1093,18 +1013,15 @@
         <v>43889</v>
       </c>
       <c r="F17">
-        <v>27912</v>
-      </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>26901</v>
+      </c>
+      <c r="G17">
+        <v>28827</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1121,18 +1038,15 @@
         <v>29873</v>
       </c>
       <c r="F18">
-        <v>31920</v>
-      </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>30596</v>
+      </c>
+      <c r="G18">
+        <v>28054</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1149,18 +1063,15 @@
         <v>116277</v>
       </c>
       <c r="F19">
-        <v>103548</v>
-      </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>103981</v>
+      </c>
+      <c r="G19">
+        <v>90824</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1177,18 +1088,15 @@
         <v>79653</v>
       </c>
       <c r="F20">
-        <v>92039</v>
-      </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <v>91923</v>
+      </c>
+      <c r="G20">
+        <v>66167</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1205,18 +1113,15 @@
         <v>13488</v>
       </c>
       <c r="F21">
-        <v>11446</v>
-      </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+        <v>11769</v>
+      </c>
+      <c r="G21">
+        <v>7478</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1233,18 +1138,15 @@
         <v>62904</v>
       </c>
       <c r="F22">
-        <v>46676</v>
-      </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+        <v>48495</v>
+      </c>
+      <c r="G22">
+        <v>36471</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1261,18 +1163,15 @@
         <v>103813</v>
       </c>
       <c r="F23">
-        <v>80345</v>
-      </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+        <v>80969</v>
+      </c>
+      <c r="G23">
+        <v>70714</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1289,18 +1188,15 @@
         <v>222207</v>
       </c>
       <c r="F24">
-        <v>134119</v>
-      </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+        <v>136707</v>
+      </c>
+      <c r="G24">
+        <v>81312</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1317,18 +1213,15 @@
         <v>93133</v>
       </c>
       <c r="F25">
-        <v>74873</v>
-      </c>
-      <c r="H25" s="5"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
-      <c r="P25" s="6"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+        <v>74829</v>
+      </c>
+      <c r="G25">
+        <v>53561</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1345,18 +1238,15 @@
         <v>45748</v>
       </c>
       <c r="F26">
+        <v>36913</v>
+      </c>
+      <c r="G26">
         <v>35843</v>
       </c>
-      <c r="H26" s="5"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="M26" s="6"/>
-      <c r="N26" s="6"/>
-      <c r="O26" s="6"/>
-      <c r="P26" s="6"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1373,18 +1263,15 @@
         <v>102126</v>
       </c>
       <c r="F27">
-        <v>52678</v>
-      </c>
-      <c r="H27" s="5"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+        <v>59602</v>
+      </c>
+      <c r="G27">
+        <v>52403</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1401,18 +1288,15 @@
         <v>14275</v>
       </c>
       <c r="F28">
-        <v>10509</v>
-      </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="M28" s="6"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+        <v>11176</v>
+      </c>
+      <c r="G28">
+        <v>6619</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1429,18 +1313,15 @@
         <v>140155</v>
       </c>
       <c r="F29">
-        <v>104515</v>
-      </c>
-      <c r="H29" s="5"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+        <v>106266</v>
+      </c>
+      <c r="G29">
+        <v>97232</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1457,18 +1338,15 @@
         <v>9502</v>
       </c>
       <c r="F30">
-        <v>9042</v>
-      </c>
-      <c r="H30" s="5"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-      <c r="P30" s="6"/>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+        <v>8065</v>
+      </c>
+      <c r="G30">
+        <v>6996</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1485,18 +1363,15 @@
         <v>16279</v>
       </c>
       <c r="F31">
-        <v>12340</v>
-      </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="M31" s="6"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="6"/>
-      <c r="P31" s="6"/>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+        <v>12222</v>
+      </c>
+      <c r="G31">
+        <v>8197</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1513,18 +1388,15 @@
         <v>25273</v>
       </c>
       <c r="F32">
-        <v>19110</v>
-      </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+        <v>20414</v>
+      </c>
+      <c r="G32">
+        <v>14347</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1541,18 +1413,15 @@
         <v>141420</v>
       </c>
       <c r="F33">
-        <v>139277</v>
-      </c>
-      <c r="H33" s="5"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+        <v>140139</v>
+      </c>
+      <c r="G33">
+        <v>71017</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1569,18 +1438,15 @@
         <v>19043</v>
       </c>
       <c r="F34">
-        <v>13338</v>
-      </c>
-      <c r="H34" s="5"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+        <v>13621</v>
+      </c>
+      <c r="G34">
+        <v>13712</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1597,18 +1463,15 @@
         <v>58641</v>
       </c>
       <c r="F35">
-        <v>40909</v>
-      </c>
-      <c r="H35" s="5"/>
-      <c r="I35" s="6"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+        <v>39496</v>
+      </c>
+      <c r="G35">
+        <v>45043</v>
+      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1625,18 +1488,15 @@
         <v>394701</v>
       </c>
       <c r="F36">
-        <v>204716</v>
-      </c>
-      <c r="H36" s="5"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+        <v>205184</v>
+      </c>
+      <c r="G36">
+        <v>218912</v>
+      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1653,18 +1513,15 @@
         <v>159317</v>
       </c>
       <c r="F37">
-        <v>108801</v>
-      </c>
-      <c r="H37" s="5"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+        <v>109830</v>
+      </c>
+      <c r="G37">
+        <v>90760</v>
+      </c>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1681,18 +1538,15 @@
         <v>54481</v>
       </c>
       <c r="F38">
-        <v>40297</v>
-      </c>
-      <c r="H38" s="5"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="5"/>
-      <c r="K38" s="5"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+        <v>46696</v>
+      </c>
+      <c r="G38">
+        <v>42577</v>
+      </c>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1709,18 +1563,15 @@
         <v>54581</v>
       </c>
       <c r="F39">
-        <v>35101</v>
-      </c>
-      <c r="H39" s="8"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+        <v>37209</v>
+      </c>
+      <c r="G39">
+        <v>46722</v>
+      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1737,18 +1588,15 @@
         <v>234868</v>
       </c>
       <c r="F40">
-        <v>198081</v>
-      </c>
-      <c r="H40" s="5"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+        <v>194594</v>
+      </c>
+      <c r="G40">
+        <v>131282</v>
+      </c>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1765,18 +1613,15 @@
         <v>42074</v>
       </c>
       <c r="F41">
-        <v>26248</v>
-      </c>
-      <c r="H41" s="5"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="5"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+        <v>26481</v>
+      </c>
+      <c r="G41">
+        <v>17087</v>
+      </c>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1793,18 +1638,15 @@
         <v>22509</v>
       </c>
       <c r="F42">
-        <v>17578</v>
-      </c>
-      <c r="H42" s="5"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="5"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+        <v>18078</v>
+      </c>
+      <c r="G42">
+        <v>13138</v>
+      </c>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1821,18 +1663,15 @@
         <v>89147</v>
       </c>
       <c r="F43">
-        <v>73116</v>
-      </c>
-      <c r="H43" s="5"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+        <v>74362</v>
+      </c>
+      <c r="G43">
+        <v>65159</v>
+      </c>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1849,18 +1688,15 @@
         <v>6359</v>
       </c>
       <c r="F44">
-        <v>5128</v>
-      </c>
-      <c r="H44" s="5"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="5"/>
-      <c r="K44" s="5"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+        <v>5295</v>
+      </c>
+      <c r="G44">
+        <v>5389</v>
+      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1877,18 +1713,15 @@
         <v>71887</v>
       </c>
       <c r="F45">
-        <v>68968</v>
-      </c>
-      <c r="H45" s="5"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="5"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+        <v>67226</v>
+      </c>
+      <c r="G45">
+        <v>43792</v>
+      </c>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1905,18 +1738,15 @@
         <v>274257</v>
       </c>
       <c r="F46">
-        <v>280406</v>
-      </c>
-      <c r="H46" s="5"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="5"/>
-      <c r="K46" s="5"/>
-      <c r="M46" s="6"/>
-      <c r="N46" s="6"/>
-      <c r="O46" s="6"/>
-      <c r="P46" s="6"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+        <v>280761</v>
+      </c>
+      <c r="G46">
+        <v>254199</v>
+      </c>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1933,18 +1763,15 @@
         <v>24515</v>
       </c>
       <c r="F47">
-        <v>19751</v>
-      </c>
-      <c r="H47" s="5"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6"/>
-      <c r="O47" s="6"/>
-      <c r="P47" s="6"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+        <v>19649</v>
+      </c>
+      <c r="G47">
+        <v>11830</v>
+      </c>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1961,18 +1788,15 @@
         <v>9662</v>
       </c>
       <c r="F48">
-        <v>6434</v>
-      </c>
-      <c r="H48" s="5"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="7"/>
-      <c r="P48" s="7"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+        <v>6598</v>
+      </c>
+      <c r="G48">
+        <v>4971</v>
+      </c>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1989,18 +1813,15 @@
         <v>6</v>
       </c>
       <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="H49" s="5"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="M49" s="6"/>
-      <c r="N49" s="6"/>
-      <c r="O49" s="6"/>
-      <c r="P49" s="6"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="G49">
+        <v>88</v>
+      </c>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -2017,18 +1838,15 @@
         <v>104619</v>
       </c>
       <c r="F50">
-        <v>84387</v>
-      </c>
-      <c r="H50" s="5"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
-      <c r="M50" s="6"/>
-      <c r="N50" s="6"/>
-      <c r="O50" s="6"/>
-      <c r="P50" s="6"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+        <v>82729</v>
+      </c>
+      <c r="G50">
+        <v>74043</v>
+      </c>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2045,18 +1863,15 @@
         <v>144455</v>
       </c>
       <c r="F51">
-        <v>89105</v>
-      </c>
-      <c r="H51" s="5"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="5"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="6"/>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+        <v>83475</v>
+      </c>
+      <c r="G51">
+        <v>145757</v>
+      </c>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2073,18 +1888,15 @@
         <v>14944</v>
       </c>
       <c r="F52">
-        <v>46251</v>
-      </c>
-      <c r="H52" s="5"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="5"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="6"/>
-      <c r="O52" s="6"/>
-      <c r="P52" s="6"/>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+        <v>46755</v>
+      </c>
+      <c r="G52">
+        <v>29576</v>
+      </c>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2101,18 +1913,15 @@
         <v>70000</v>
       </c>
       <c r="F53">
-        <v>55886</v>
-      </c>
-      <c r="H53" s="5"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="5"/>
-      <c r="M53" s="6"/>
-      <c r="N53" s="6"/>
-      <c r="O53" s="6"/>
-      <c r="P53" s="6"/>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+        <v>55883</v>
+      </c>
+      <c r="G53">
+        <v>49910</v>
+      </c>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2129,48 +1938,37 @@
         <v>5794</v>
       </c>
       <c r="F54">
-        <v>3321</v>
-      </c>
-      <c r="I54" s="2"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="4"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K55" s="2"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="4"/>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K56" s="2"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="4"/>
+        <v>4381</v>
+      </c>
+      <c r="G54">
+        <v>2886</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Include updated WA/NY data
- We will be using BLS data for update, but we update WA/NY data in case anyone wants to run those numbers
- Update readme with more detailed manual data update instructions
</commit_message>
<xml_diff>
--- a/data/raw-data/small/initial-claims-bls-state.xlsx
+++ b/data/raw-data/small/initial-claims-bls-state.xlsx
@@ -197,9 +197,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0;#,##0"/>
-    <numFmt numFmtId="165" formatCode="###0;###0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -236,13 +235,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -586,14 +582,14 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -618,7 +614,9 @@
       <c r="G1" s="1">
         <v>43946</v>
       </c>
-      <c r="H1" s="2"/>
+      <c r="H1" s="1">
+        <v>43952</v>
+      </c>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -641,10 +639,11 @@
         <v>66432</v>
       </c>
       <c r="G2">
-        <v>64170</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+        <v>74966</v>
+      </c>
+      <c r="H2">
+        <v>28183</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -666,10 +665,11 @@
         <v>12201</v>
       </c>
       <c r="G3">
-        <v>1187</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+        <v>10313</v>
+      </c>
+      <c r="H3">
+        <v>9404</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -691,10 +691,11 @@
         <v>25404</v>
       </c>
       <c r="G4">
-        <v>16745</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+        <v>17671</v>
+      </c>
+      <c r="H4">
+        <v>12436</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -716,10 +717,11 @@
         <v>72457</v>
       </c>
       <c r="G5">
-        <v>52098</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+        <v>52581</v>
+      </c>
+      <c r="H5">
+        <v>42909</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -741,10 +743,11 @@
         <v>528360</v>
       </c>
       <c r="G6">
-        <v>328042</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+        <v>325343</v>
+      </c>
+      <c r="H6">
+        <v>318064</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -766,10 +769,11 @@
         <v>67639</v>
       </c>
       <c r="G7">
-        <v>38367</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+        <v>38662</v>
+      </c>
+      <c r="H7">
+        <v>28322</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -791,10 +795,11 @@
         <v>102808</v>
       </c>
       <c r="G8">
-        <v>33037</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+        <v>33041</v>
+      </c>
+      <c r="H8">
+        <v>36166</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -816,10 +821,11 @@
         <v>9446</v>
       </c>
       <c r="G9">
-        <v>7754</v>
-      </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+        <v>7947</v>
+      </c>
+      <c r="H9">
+        <v>6183</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -841,10 +847,11 @@
         <v>8639</v>
       </c>
       <c r="G10">
-        <v>8158</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+        <v>8708</v>
+      </c>
+      <c r="H10">
+        <v>8133</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -866,10 +873,11 @@
         <v>506670</v>
       </c>
       <c r="G11">
-        <v>432465</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+        <v>433103</v>
+      </c>
+      <c r="H11">
+        <v>173191</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -891,10 +899,11 @@
         <v>247003</v>
       </c>
       <c r="G12">
-        <v>264818</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+        <v>266565</v>
+      </c>
+      <c r="H12">
+        <v>226884</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -916,10 +925,11 @@
         <v>26591</v>
       </c>
       <c r="G13">
-        <v>22615</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+        <v>22495</v>
+      </c>
+      <c r="H13">
+        <v>16112</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -941,10 +951,11 @@
         <v>13023</v>
       </c>
       <c r="G14">
-        <v>8268</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+        <v>8827</v>
+      </c>
+      <c r="H14">
+        <v>7194</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -966,10 +977,11 @@
         <v>102936</v>
       </c>
       <c r="G15">
-        <v>81245</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+        <v>81596</v>
+      </c>
+      <c r="H15">
+        <v>74476</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -991,12 +1003,13 @@
         <v>72756</v>
       </c>
       <c r="G16">
-        <v>57397</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>55774</v>
+      </c>
+      <c r="H16">
+        <v>43777</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1016,12 +1029,13 @@
         <v>26901</v>
       </c>
       <c r="G17">
-        <v>28827</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>27220</v>
+      </c>
+      <c r="H17">
+        <v>24693</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1041,12 +1055,13 @@
         <v>30596</v>
       </c>
       <c r="G18">
-        <v>28054</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>24483</v>
+      </c>
+      <c r="H18">
+        <v>18281</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1066,12 +1081,13 @@
         <v>103981</v>
       </c>
       <c r="G19">
-        <v>90824</v>
-      </c>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>91223</v>
+      </c>
+      <c r="H19">
+        <v>80060</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1091,12 +1107,13 @@
         <v>91923</v>
       </c>
       <c r="G20">
-        <v>66167</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>66141</v>
+      </c>
+      <c r="H20">
+        <v>52137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1116,12 +1133,13 @@
         <v>11769</v>
       </c>
       <c r="G21">
-        <v>7478</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>7661</v>
+      </c>
+      <c r="H21">
+        <v>16175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1141,12 +1159,13 @@
         <v>48495</v>
       </c>
       <c r="G22">
-        <v>36471</v>
-      </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>37925</v>
+      </c>
+      <c r="H22">
+        <v>65262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1166,12 +1185,13 @@
         <v>80969</v>
       </c>
       <c r="G23">
-        <v>70714</v>
-      </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+        <v>71358</v>
+      </c>
+      <c r="H23">
+        <v>55448</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1191,12 +1211,13 @@
         <v>136707</v>
       </c>
       <c r="G24">
-        <v>81312</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+        <v>82004</v>
+      </c>
+      <c r="H24">
+        <v>68952</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1216,12 +1237,13 @@
         <v>74829</v>
       </c>
       <c r="G25">
-        <v>53561</v>
-      </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>48595</v>
+      </c>
+      <c r="H25">
+        <v>47134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1241,12 +1263,13 @@
         <v>36913</v>
       </c>
       <c r="G26">
-        <v>35843</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>29906</v>
+      </c>
+      <c r="H26">
+        <v>24810</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1266,12 +1289,13 @@
         <v>59602</v>
       </c>
       <c r="G27">
-        <v>52403</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+        <v>55299</v>
+      </c>
+      <c r="H27">
+        <v>49402</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1291,12 +1315,13 @@
         <v>11176</v>
       </c>
       <c r="G28">
-        <v>6619</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>7052</v>
+      </c>
+      <c r="H28">
+        <v>4263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1316,12 +1341,13 @@
         <v>106266</v>
       </c>
       <c r="G29">
-        <v>97232</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+        <v>98941</v>
+      </c>
+      <c r="H29">
+        <v>84716</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1341,12 +1367,13 @@
         <v>8065</v>
       </c>
       <c r="G30">
-        <v>6996</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+        <v>6274</v>
+      </c>
+      <c r="H30">
+        <v>4689</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1366,12 +1393,13 @@
         <v>12222</v>
       </c>
       <c r="G31">
-        <v>8197</v>
-      </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+        <v>8229</v>
+      </c>
+      <c r="H31">
+        <v>6555</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1391,12 +1419,13 @@
         <v>20414</v>
       </c>
       <c r="G32">
-        <v>14347</v>
-      </c>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+        <v>15001</v>
+      </c>
+      <c r="H32">
+        <v>11834</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1416,12 +1445,13 @@
         <v>140139</v>
       </c>
       <c r="G33">
-        <v>71017</v>
-      </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+        <v>71966</v>
+      </c>
+      <c r="H33">
+        <v>87540</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1441,12 +1471,13 @@
         <v>13621</v>
       </c>
       <c r="G34">
-        <v>13712</v>
-      </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+        <v>12093</v>
+      </c>
+      <c r="H34">
+        <v>16801</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1466,12 +1497,13 @@
         <v>39496</v>
       </c>
       <c r="G35">
-        <v>45043</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+        <v>42541</v>
+      </c>
+      <c r="H35">
+        <v>30735</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1491,12 +1523,13 @@
         <v>205184</v>
       </c>
       <c r="G36">
-        <v>218912</v>
-      </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+        <v>219413</v>
+      </c>
+      <c r="H36">
+        <v>195242</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1516,12 +1549,13 @@
         <v>109830</v>
       </c>
       <c r="G37">
-        <v>90760</v>
-      </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+        <v>93599</v>
+      </c>
+      <c r="H37">
+        <v>61046</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1541,12 +1575,13 @@
         <v>46696</v>
       </c>
       <c r="G38">
-        <v>42577</v>
-      </c>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+        <v>52500</v>
+      </c>
+      <c r="H38">
+        <v>68237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1566,12 +1601,13 @@
         <v>37209</v>
       </c>
       <c r="G39">
-        <v>46722</v>
-      </c>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+        <v>49300</v>
+      </c>
+      <c r="H39">
+        <v>45102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1591,12 +1627,13 @@
         <v>194594</v>
       </c>
       <c r="G40">
-        <v>131282</v>
-      </c>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+        <v>127896</v>
+      </c>
+      <c r="H40">
+        <v>96603</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1616,12 +1653,13 @@
         <v>26481</v>
       </c>
       <c r="G41">
-        <v>17087</v>
-      </c>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+        <v>17286</v>
+      </c>
+      <c r="H41">
+        <v>21673</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1641,12 +1679,13 @@
         <v>18078</v>
       </c>
       <c r="G42">
-        <v>13138</v>
-      </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+        <v>13084</v>
+      </c>
+      <c r="H42">
+        <v>9109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1666,12 +1705,13 @@
         <v>74362</v>
       </c>
       <c r="G43">
-        <v>65159</v>
-      </c>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+        <v>66438</v>
+      </c>
+      <c r="H43">
+        <v>46747</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1691,12 +1731,13 @@
         <v>5295</v>
       </c>
       <c r="G44">
-        <v>5389</v>
-      </c>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+        <v>5535</v>
+      </c>
+      <c r="H44">
+        <v>3756</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1716,12 +1757,13 @@
         <v>67226</v>
       </c>
       <c r="G45">
-        <v>43792</v>
-      </c>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+        <v>42805</v>
+      </c>
+      <c r="H45">
+        <v>37319</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1741,12 +1783,13 @@
         <v>280761</v>
       </c>
       <c r="G46">
-        <v>254199</v>
-      </c>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+        <v>254084</v>
+      </c>
+      <c r="H46">
+        <v>247179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1766,12 +1809,13 @@
         <v>19649</v>
       </c>
       <c r="G47">
-        <v>11830</v>
-      </c>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+        <v>11738</v>
+      </c>
+      <c r="H47">
+        <v>9057</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1791,12 +1835,13 @@
         <v>6598</v>
       </c>
       <c r="G48">
-        <v>4971</v>
-      </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+        <v>5117</v>
+      </c>
+      <c r="H48">
+        <v>3759</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1816,12 +1861,13 @@
         <v>13</v>
       </c>
       <c r="G49">
-        <v>88</v>
-      </c>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+      <c r="H49">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1841,12 +1887,13 @@
         <v>82729</v>
       </c>
       <c r="G50">
-        <v>74043</v>
-      </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+        <v>72488</v>
+      </c>
+      <c r="H50">
+        <v>61138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1866,12 +1913,13 @@
         <v>83475</v>
       </c>
       <c r="G51">
-        <v>145757</v>
-      </c>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+        <v>139505</v>
+      </c>
+      <c r="H51">
+        <v>109167</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1891,12 +1939,13 @@
         <v>46755</v>
       </c>
       <c r="G52">
-        <v>29576</v>
-      </c>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+        <v>29818</v>
+      </c>
+      <c r="H52">
+        <v>12996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -1916,12 +1965,13 @@
         <v>55883</v>
       </c>
       <c r="G53">
-        <v>49910</v>
-      </c>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+        <v>49993</v>
+      </c>
+      <c r="H53">
+        <v>38002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -1941,7 +1991,10 @@
         <v>4381</v>
       </c>
       <c r="G54">
-        <v>2886</v>
+        <v>3497</v>
+      </c>
+      <c r="H54">
+        <v>2026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>